<commit_message>
Excelsheet update en comment line in au3
</commit_message>
<xml_diff>
--- a/Hulp-schema-calc-new.xlsx
+++ b/Hulp-schema-calc-new.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Pathingtest\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
   <si>
     <t>14 = goal</t>
   </si>
@@ -200,19 +200,40 @@
     <t>recht</t>
   </si>
   <si>
-    <t>linkonder-rechtsboven</t>
-  </si>
-  <si>
-    <t>linkboven-rechtsonder</t>
-  </si>
-  <si>
-    <t>rechtsonder-linksboven</t>
-  </si>
-  <si>
-    <t>rechtsboven-linksonder</t>
-  </si>
-  <si>
-    <t>V</t>
+    <t>ABS(startx-goalx)</t>
+  </si>
+  <si>
+    <t>ABS(starty-goaly)</t>
+  </si>
+  <si>
+    <t>ABS(x - y)</t>
+  </si>
+  <si>
+    <t>(x+y-(ABS(x - y)))/2</t>
+  </si>
+  <si>
+    <t>Horizontal/Vertical</t>
+  </si>
+  <si>
+    <t>Diagonal</t>
+  </si>
+  <si>
+    <t>abs(abs(startX - goalX) - abs(startY - goalY))</t>
+  </si>
+  <si>
+    <t>hori diff</t>
+  </si>
+  <si>
+    <t>verti diff</t>
+  </si>
+  <si>
+    <t>=hori movement</t>
+  </si>
+  <si>
+    <t>=verti movement</t>
+  </si>
+  <si>
+    <t>abs(startX-goalX) + abs(startY - goalY) - abs(abs(startX - goalX) - abs(startY - goalY))) / 2</t>
   </si>
 </sst>
 </file>
@@ -375,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,11 +433,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -729,7 +824,7 @@
   <dimension ref="A1:AM79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="AJ66" sqref="AJ66"/>
+      <selection activeCell="AB77" sqref="AB77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,6 +836,7 @@
     <col min="12" max="12" width="3" customWidth="1"/>
     <col min="13" max="13" width="3.140625" customWidth="1"/>
     <col min="14" max="26" width="3" customWidth="1"/>
+    <col min="28" max="28" width="33.7109375" customWidth="1"/>
     <col min="29" max="29" width="17.28515625" customWidth="1"/>
     <col min="34" max="34" width="12.140625" customWidth="1"/>
     <col min="36" max="36" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -1335,7 +1431,7 @@
       <c r="B56" s="3">
         <v>1</v>
       </c>
-      <c r="C56" s="12">
+      <c r="C56" s="10">
         <v>2</v>
       </c>
       <c r="D56" s="1">
@@ -1349,6 +1445,14 @@
       </c>
       <c r="H56">
         <v>1</v>
+      </c>
+      <c r="K56" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20">
+        <v>2</v>
       </c>
       <c r="AC56" s="14" t="s">
         <v>22</v>
@@ -1373,10 +1477,10 @@
       <c r="AM56" s="13"/>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B57" s="12">
+      <c r="B57" s="10">
         <v>6</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="16">
         <v>7</v>
       </c>
       <c r="D57" s="10">
@@ -1389,6 +1493,14 @@
         <v>10</v>
       </c>
       <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="K57" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20">
         <v>2</v>
       </c>
       <c r="AC57" s="14" t="s">
@@ -1426,11 +1538,19 @@
       <c r="E58" s="10">
         <v>14</v>
       </c>
-      <c r="F58" s="16">
+      <c r="F58" s="1">
         <v>15</v>
       </c>
       <c r="H58">
         <v>3</v>
+      </c>
+      <c r="K58" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19">
+        <v>5</v>
       </c>
       <c r="AC58" s="14" t="s">
         <v>24</v>
@@ -1464,13 +1584,21 @@
       <c r="D59" s="2">
         <v>18</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="1">
         <v>19</v>
       </c>
       <c r="F59" s="10">
         <v>20</v>
       </c>
       <c r="H59">
+        <v>4</v>
+      </c>
+      <c r="K59" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19">
         <v>4</v>
       </c>
       <c r="AC59" s="14" t="s">
@@ -1508,7 +1636,7 @@
       <c r="D60" s="1">
         <v>23</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="15">
         <v>24</v>
       </c>
       <c r="F60" s="3">
@@ -1591,12 +1719,17 @@
       <c r="AM62" s="13"/>
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="L63" t="s">
+      <c r="B63">
+        <f>ABS(N57-N59)</f>
+        <v>2</v>
+      </c>
+      <c r="D63" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="T63" s="17" t="s">
-        <v>62</v>
-      </c>
+      <c r="J63" t="s">
+        <v>65</v>
+      </c>
+      <c r="T63" s="17"/>
       <c r="AC63" s="14" t="s">
         <v>47</v>
       </c>
@@ -1622,12 +1755,17 @@
       <c r="AM63" s="13"/>
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="L64" t="s">
+      <c r="B64">
+        <f>ABS(N56-N58)</f>
+        <v>3</v>
+      </c>
+      <c r="D64" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="T64" s="17" t="s">
-        <v>62</v>
-      </c>
+      <c r="J64" t="s">
+        <v>66</v>
+      </c>
+      <c r="T64" s="17"/>
       <c r="AC64" s="14"/>
       <c r="AD64" s="14"/>
       <c r="AE64" s="14"/>
@@ -1638,13 +1776,8 @@
       <c r="AL64" s="13"/>
       <c r="AM64" s="13"/>
     </row>
-    <row r="65" spans="12:39" x14ac:dyDescent="0.25">
-      <c r="L65" t="s">
-        <v>60</v>
-      </c>
-      <c r="T65" s="17" t="s">
-        <v>62</v>
-      </c>
+    <row r="65" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="T65" s="17"/>
       <c r="AC65" s="14" t="s">
         <v>48</v>
       </c>
@@ -1671,13 +1804,18 @@
       </c>
       <c r="AM65" s="13"/>
     </row>
-    <row r="66" spans="12:39" x14ac:dyDescent="0.25">
-      <c r="L66" t="s">
-        <v>61</v>
-      </c>
-      <c r="T66" s="17" t="s">
-        <v>62</v>
-      </c>
+    <row r="66" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <f>ABS(B63-B64)</f>
+        <v>1</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J66" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T66" s="17"/>
       <c r="AC66" s="14" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1842,17 @@
       </c>
       <c r="AM66" s="13"/>
     </row>
-    <row r="67" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <f>((B63+B64)-B66)/2</f>
+        <v>2</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J67" s="18" t="s">
+        <v>68</v>
+      </c>
       <c r="AH67" s="13"/>
       <c r="AI67" s="13"/>
       <c r="AJ67" s="13"/>
@@ -1712,7 +1860,7 @@
       <c r="AL67" s="13"/>
       <c r="AM67" s="13"/>
     </row>
-    <row r="68" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH68" s="13"/>
       <c r="AI68" s="13"/>
       <c r="AJ68" s="13"/>
@@ -1720,7 +1868,7 @@
       <c r="AL68" s="13"/>
       <c r="AM68" s="13"/>
     </row>
-    <row r="69" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH69" s="13"/>
       <c r="AI69" s="13"/>
       <c r="AJ69" s="13"/>
@@ -1728,7 +1876,17 @@
       <c r="AL69" s="13"/>
       <c r="AM69" s="13"/>
     </row>
-    <row r="70" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70">
+        <f>(ABS(N57-N59) + ABS(N56 - N58) -  ABS(ABS(N57 - N59) - ABS(N56 - N58))) / 2</f>
+        <v>2</v>
+      </c>
+      <c r="I70" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="AH70" s="13"/>
       <c r="AI70" s="13"/>
       <c r="AJ70" s="13"/>
@@ -1736,7 +1894,17 @@
       <c r="AL70" s="13"/>
       <c r="AM70" s="13"/>
     </row>
-    <row r="71" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>62</v>
+      </c>
+      <c r="H71">
+        <f>ABS(ABS(N57-N59)-ABS(N56-N58))</f>
+        <v>1</v>
+      </c>
+      <c r="I71" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="AH71" s="13" t="s">
         <v>49</v>
       </c>
@@ -1746,7 +1914,7 @@
       <c r="AL71" s="13"/>
       <c r="AM71" s="13"/>
     </row>
-    <row r="72" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH72" s="13"/>
       <c r="AI72" s="13"/>
       <c r="AJ72" s="13"/>
@@ -1754,7 +1922,7 @@
       <c r="AL72" s="13"/>
       <c r="AM72" s="13"/>
     </row>
-    <row r="73" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH73" s="13"/>
       <c r="AI73" s="13"/>
       <c r="AJ73" s="13"/>
@@ -1762,7 +1930,7 @@
       <c r="AL73" s="13"/>
       <c r="AM73" s="13"/>
     </row>
-    <row r="74" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH74" s="13" t="s">
         <v>50</v>
       </c>
@@ -1775,7 +1943,7 @@
       <c r="AL74" s="13"/>
       <c r="AM74" s="13"/>
     </row>
-    <row r="75" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH75" s="13"/>
       <c r="AI75" s="13"/>
       <c r="AJ75" s="13"/>
@@ -1783,7 +1951,7 @@
       <c r="AL75" s="13"/>
       <c r="AM75" s="13"/>
     </row>
-    <row r="76" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH76" s="13"/>
       <c r="AI76" s="13"/>
       <c r="AJ76" s="13"/>
@@ -1791,7 +1959,7 @@
       <c r="AL76" s="13"/>
       <c r="AM76" s="13"/>
     </row>
-    <row r="77" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH77" s="13" t="s">
         <v>55</v>
       </c>
@@ -1804,7 +1972,7 @@
       <c r="AL77" s="13"/>
       <c r="AM77" s="13"/>
     </row>
-    <row r="78" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH78" s="13" t="s">
         <v>56</v>
       </c>
@@ -1817,7 +1985,7 @@
       <c r="AL78" s="13"/>
       <c r="AM78" s="13"/>
     </row>
-    <row r="79" spans="12:39" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:39" x14ac:dyDescent="0.25">
       <c r="AH79" s="13" t="s">
         <v>54</v>
       </c>
@@ -1831,6 +1999,16 @@
       <c r="AM79" s="13"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B56">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND($N$56=1,$N$57=1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND($N$56=1,$N$57=2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>